<commit_message>
fixed loop, found inconsistencies in data
social files without practice runs were missing three columns between 'amount' and 'probability'
</commit_message>
<xml_diff>
--- a/data/social/S_1011.xlsx
+++ b/data/social/S_1011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-effort/data/social/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6AE9EC-2B3D-8B4D-BFC3-A054072F487B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30CA2EC-7975-FA40-8B9A-F8E19F1A48F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="15380" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44800" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S_1009" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="33">
   <si>
     <t>ExperimentName</t>
   </si>
@@ -962,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI68"/>
+  <dimension ref="A1:AI67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A41" sqref="A1:I68"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6348,84 +6348,9 @@
       <c r="I51">
         <v>0</v>
       </c>
-      <c r="J51" t="s">
-        <v>26</v>
-      </c>
-      <c r="K51">
-        <v>1011</v>
-      </c>
-      <c r="L51">
-        <v>71</v>
-      </c>
-      <c r="M51" t="s">
-        <v>31</v>
-      </c>
-      <c r="N51">
-        <v>60.01</v>
-      </c>
-      <c r="O51">
-        <v>1</v>
-      </c>
-      <c r="P51">
-        <v>560399613</v>
-      </c>
-      <c r="Q51" s="1">
-        <v>43878</v>
-      </c>
-      <c r="R51" s="2">
-        <v>43878.718969907408</v>
-      </c>
-      <c r="S51" s="3">
-        <v>0.51063657407407403</v>
-      </c>
-      <c r="T51">
-        <v>50</v>
-      </c>
-      <c r="U51" t="s">
-        <v>32</v>
-      </c>
-      <c r="V51" t="s">
-        <v>32</v>
-      </c>
-      <c r="W51" t="s">
-        <v>32</v>
-      </c>
-      <c r="X51" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y51" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z51" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA51" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB51" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC51" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD51" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE51" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF51">
-        <v>46</v>
-      </c>
-      <c r="AG51" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH51" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI51" t="s">
-        <v>32</v>
-      </c>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="3"/>
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A52">
@@ -6843,7 +6768,7 @@
       <c r="Z64" s="2"/>
       <c r="AA64" s="3"/>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>0</v>
       </c>
@@ -6871,11 +6796,8 @@
       <c r="I65">
         <v>0</v>
       </c>
-      <c r="Y65" s="1"/>
-      <c r="Z65" s="2"/>
-      <c r="AA65" s="3"/>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>0</v>
       </c>
@@ -6904,7 +6826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>0</v>
       </c>
@@ -6930,35 +6852,6 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>0</v>
-      </c>
-      <c r="B68">
-        <v>0</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
turning off hline @ line 110 works on my computer
</commit_message>
<xml_diff>
--- a/data/social/S_1011.xlsx
+++ b/data/social/S_1011.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/GitHub/istart-effort/data/social/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30CA2EC-7975-FA40-8B9A-F8E19F1A48F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E1561E-EA28-704B-B326-53BA533E0489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44800" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20300" yWindow="2600" windowWidth="19760" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S_1009" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="42">
   <si>
     <t>ExperimentName</t>
   </si>
@@ -119,6 +119,33 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>AmtWon</t>
+  </si>
+  <si>
+    <t>Clock.Information</t>
+  </si>
+  <si>
+    <t>EasyKey</t>
+  </si>
+  <si>
+    <t>ExperimentVersion</t>
+  </si>
+  <si>
+    <t>HardKey</t>
+  </si>
+  <si>
+    <t>RuntimeCapabilities</t>
+  </si>
+  <si>
+    <t>RuntimeVersion</t>
+  </si>
+  <si>
+    <t>RuntimeVersionExpected</t>
+  </si>
+  <si>
+    <t>StudioVersion</t>
   </si>
 </sst>
 </file>
@@ -964,69 +991,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>0</v>
-      </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="L1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="N1" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="P1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="T1" t="s">
         <v>10</v>

</xml_diff>